<commit_message>
messed around with day of week priority.  Max game limit is working well.  Max late games is not working well
</commit_message>
<xml_diff>
--- a/data/League-2019-07-26.xlsx
+++ b/data/League-2019-07-26.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Downloads\League Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\DjangoLeagueScheduler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E932663B-1E53-44E9-9EB8-C72DB1D6F4DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BC4EF9-3BB1-4F06-BD7C-98D01425CE05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30915" yWindow="2250" windowWidth="21600" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablib Dataset" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -62,6 +62,48 @@
   </si>
   <si>
     <t>CoachPitch</t>
+  </si>
+  <si>
+    <t>maxLateGames</t>
+  </si>
+  <si>
+    <t>maxGames</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -80,6 +122,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,7 +145,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -407,93 +451,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added coach affiliation, coach overlap, better import, updated models to support Slot first approach, handicap, double round robin - and other stuff
need to focus on secondary league per slot
</commit_message>
<xml_diff>
--- a/data/League-2019-07-26.xlsx
+++ b/data/League-2019-07-26.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\DjangoLeagueScheduler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BC4EF9-3BB1-4F06-BD7C-98D01425CE05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E82E66A-0FD4-4360-ACE0-66F68F7D070D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -82,13 +82,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>14</t>
-  </si>
-  <si>
     <t>3</t>
-  </si>
-  <si>
-    <t>8</t>
   </si>
   <si>
     <t>2</t>
@@ -455,7 +449,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -494,8 +488,8 @@
       <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
+      <c r="F2" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -509,11 +503,11 @@
         <v>11</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="1">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1">
         <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -530,13 +524,13 @@
       <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
+      <c r="F4" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -548,31 +542,31 @@
       <c r="E5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
+      <c r="F5" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="F6" s="1">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -581,13 +575,13 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>